<commit_message>
added a lot more code, cleaned versions of dataframes
</commit_message>
<xml_diff>
--- a/residential-nonresidential-fire-loss-estimates-2003-2021_fixed.xlsx
+++ b/residential-nonresidential-fire-loss-estimates-2003-2021_fixed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saumyagupta/Documents/j233/final_project/j233_final_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9362B42-4575-FC41-8AF2-09BC6EBBB419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6D5ACE-5BF2-6A43-996F-E8D257DA1D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29600" windowHeight="18600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29600" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Res Bldg Prop Typ Est 2003-2021" sheetId="15" r:id="rId1"/>
@@ -378,1075 +378,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="90">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1761,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC981BD8-0A34-4F47-95E1-4663C8FAD525}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2607,7 +1539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5527F1D5-C82F-0B44-8499-6A88A697893E}">
   <dimension ref="A1:AU20"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
@@ -8289,228 +7221,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B20">
-    <cfRule type="cellIs" dxfId="89" priority="45" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E20">
-    <cfRule type="cellIs" dxfId="88" priority="44" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H20">
-    <cfRule type="cellIs" dxfId="87" priority="43" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K20">
-    <cfRule type="cellIs" dxfId="86" priority="42" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N20">
-    <cfRule type="cellIs" dxfId="85" priority="41" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q20">
-    <cfRule type="cellIs" dxfId="84" priority="40" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T20">
-    <cfRule type="cellIs" dxfId="83" priority="39" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W2:W20">
-    <cfRule type="cellIs" dxfId="82" priority="38" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z2:Z20">
-    <cfRule type="cellIs" dxfId="81" priority="37" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC20">
-    <cfRule type="cellIs" dxfId="80" priority="36" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF2:AF20">
-    <cfRule type="cellIs" dxfId="79" priority="35" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI2:AI20">
-    <cfRule type="cellIs" dxfId="78" priority="34" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL2:AL20">
-    <cfRule type="cellIs" dxfId="77" priority="33" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO2:AO20">
-    <cfRule type="cellIs" dxfId="76" priority="32" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR2:AR20">
-    <cfRule type="cellIs" dxfId="75" priority="31" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C20">
-    <cfRule type="cellIs" dxfId="74" priority="30" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F20">
-    <cfRule type="cellIs" dxfId="73" priority="29" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I20">
-    <cfRule type="cellIs" dxfId="72" priority="28" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L20">
-    <cfRule type="cellIs" dxfId="71" priority="27" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O20">
-    <cfRule type="cellIs" dxfId="70" priority="26" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R20">
-    <cfRule type="cellIs" dxfId="69" priority="25" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U20">
-    <cfRule type="cellIs" dxfId="68" priority="24" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X20">
-    <cfRule type="cellIs" dxfId="67" priority="23" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA2:AA20">
-    <cfRule type="cellIs" dxfId="66" priority="22" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD2:AD20">
-    <cfRule type="cellIs" dxfId="65" priority="21" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG2:AG20">
-    <cfRule type="cellIs" dxfId="64" priority="20" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ2:AJ20">
-    <cfRule type="cellIs" dxfId="63" priority="19" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM2:AM20">
-    <cfRule type="cellIs" dxfId="62" priority="18" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP2:AP20">
-    <cfRule type="cellIs" dxfId="61" priority="17" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AS2:AS20">
-    <cfRule type="cellIs" dxfId="60" priority="16" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D20">
-    <cfRule type="cellIs" dxfId="59" priority="15" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
-    <cfRule type="cellIs" dxfId="58" priority="14" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J20">
-    <cfRule type="cellIs" dxfId="57" priority="13" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M20">
-    <cfRule type="cellIs" dxfId="56" priority="12" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P20">
-    <cfRule type="cellIs" dxfId="55" priority="11" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S20">
-    <cfRule type="cellIs" dxfId="54" priority="10" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V2:V20">
-    <cfRule type="cellIs" dxfId="53" priority="9" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y20">
-    <cfRule type="cellIs" dxfId="52" priority="8" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB2:AB20">
-    <cfRule type="cellIs" dxfId="51" priority="7" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE2:AE20">
-    <cfRule type="cellIs" dxfId="50" priority="6" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH2:AH20">
-    <cfRule type="cellIs" dxfId="49" priority="5" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK2:AK20">
-    <cfRule type="cellIs" dxfId="48" priority="4" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN2:AN20">
-    <cfRule type="cellIs" dxfId="47" priority="3" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ2:AQ20">
-    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
-      <formula>"0*"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AT2:AT20">
-    <cfRule type="cellIs" dxfId="45" priority="1" operator="equal">
+  <conditionalFormatting sqref="B2:AT20">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"0*"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11337,7 +10049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12FE71FA-FBBE-AB47-AD61-B3CEE280180C}">
   <dimension ref="A1:AT20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>

</xml_diff>